<commit_message>
pushing fix for dynamic content loader
</commit_message>
<xml_diff>
--- a/job-data.xlsx
+++ b/job-data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,306 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>RPA Developer</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-rpa-developer-dautom-bengaluru-2-to-6-years-170524500436</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Automation Anywhere Developer</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-automation-anywhere-developer-ilink-digital-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-2-to-4-years-170524500687</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>RPA Business Analyst</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-rpa-business-analyst-percipere-mumbai-pune-0-to-1-years-170524909865</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Senior RPA Business Analyst</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-senior-rpa-business-analyst-percipere-mumbai-5-to-7-years-170524909645</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rpa Developer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-rpa-developer-apmosys-technologies-navi-mumbai-8-to-10-years-170524008223</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Opportunity For RPA Developers</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-opportunity-for-rpa-developers-healthcare-informatics-vadodara-2-to-5-years-250424004964</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RPA Support Specialist (Night Shift, US Hours)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-rpa-support-specialist-night-shift-us-hours-percipere-mumbai-2-to-3-years-170524912102</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RPA diversity opening For Ahmedabad Location</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-rpa-diversity-opening-for-ahmedabad-location-infosys-bpm-ahmedabad-6-to-10-years-030424012572</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Senior Developer</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-senior-developer-acronotics-pvt-ltd-pune-bengaluru-5-to-10-years-170524500545</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-developer-acronotics-pvt-ltd-pune-bengaluru-3-to-8-years-170524500544</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Solution Architects</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-solution-architects-acronotics-pvt-ltd-pune-bengaluru-8-to-13-years-170524500638</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RPA  Robot Framework &amp; Python QA Automation</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-rpa-robot-framework-python-qa-automation-rq-technologies-llp-chennai-5-to-10-years-170524011474</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Application Developer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-mumbai-3-to-5-years-170524908871</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Application Developer</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-3-to-6-years-170524904578</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Technical BotOps</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-technical-botops-allegis-group-hyderabad-1-to-5-years-170524004542</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Application Designer</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-application-designer-accenture-solutions-pvt-ltd-bengaluru-3-to-5-years-170524912002</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Application Designer</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-application-designer-accenture-solutions-pvt-ltd-bengaluru-3-to-7-years-170524911413</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Application Designer</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-application-designer-accenture-solutions-pvt-ltd-bengaluru-7-to-9-years-170524912884</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Trust &amp; Safety New Associate</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-trust-safety-new-associate-accenture-solutions-pvt-ltd-gurugram-0-to-1-years-180524908538</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>S&amp;C Global Network - Strategy - MC - Industry X - Capital Projects</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-s-c-global-network-strategy-mc-industry-x-capital-projects-accenture-solutions-pvt-ltd-gurugram-7-to-9-years-170524908957</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added a feature to fetch job details and description
</commit_message>
<xml_diff>
--- a/job-data.xlsx
+++ b/job-data.xlsx
@@ -451,12 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RPA Developer</t>
+          <t>RPA Uipath Developer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-rpa-developer-dautom-bengaluru-2-to-6-years-170524500436</t>
+          <t>https://www.naukri.com/job-listings-rpa-uipath-developer-semperfi-solutions-bengaluru-13-to-15-years-190524902070</t>
         </is>
       </c>
     </row>
@@ -466,12 +466,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Automation Anywhere Developer</t>
+          <t>RPA Developer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-automation-anywhere-developer-ilink-digital-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-2-to-4-years-170524500687</t>
+          <t>https://www.naukri.com/job-listings-rpa-developer-percipere-mumbai-0-to-1-years-190524902221</t>
         </is>
       </c>
     </row>
@@ -481,12 +481,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RPA Business Analyst</t>
+          <t>Application Automation Engineer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-rpa-business-analyst-percipere-mumbai-pune-0-to-1-years-170524909865</t>
+          <t>https://www.naukri.com/job-listings-application-automation-engineer-accenture-solutions-pvt-ltd-pune-3-to-5-years-190524901638</t>
         </is>
       </c>
     </row>
@@ -496,12 +496,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Senior RPA Business Analyst</t>
+          <t>Service Management New Associate - Automation and Analytics</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-senior-rpa-business-analyst-percipere-mumbai-5-to-7-years-170524909645</t>
+          <t>https://www.naukri.com/job-listings-service-management-new-associate-automation-and-analytics-accenture-solutions-pvt-ltd-bengaluru-0-to-1-years-190524901762</t>
         </is>
       </c>
     </row>
@@ -511,12 +511,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rpa Developer</t>
+          <t>Trust &amp; Safety New Associate</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-rpa-developer-apmosys-technologies-navi-mumbai-8-to-10-years-170524008223</t>
+          <t>https://www.naukri.com/job-listings-trust-safety-new-associate-accenture-solutions-pvt-ltd-gurugram-0-to-1-years-180524908538</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Opportunity For RPA Developers</t>
+          <t>BPM Consultant</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-opportunity-for-rpa-developers-healthcare-informatics-vadodara-2-to-5-years-250424004964</t>
+          <t>https://www.naukri.com/job-listings-bpm-consultant-percipere-mumbai-7-to-11-years-180524906883</t>
         </is>
       </c>
     </row>
@@ -541,12 +541,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RPA Support Specialist (Night Shift, US Hours)</t>
+          <t>Insurance Operations Manager</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-rpa-support-specialist-night-shift-us-hours-percipere-mumbai-2-to-3-years-170524912102</t>
+          <t>https://www.naukri.com/job-listings-insurance-operations-manager-accenture-solutions-pvt-ltd-hyderabad-16-to-25-years-180524903816</t>
         </is>
       </c>
     </row>
@@ -556,12 +556,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RPA diversity opening For Ahmedabad Location</t>
+          <t>Application Developer</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-rpa-diversity-opening-for-ahmedabad-location-infosys-bpm-ahmedabad-6-to-10-years-030424012572</t>
+          <t>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-mumbai-3-to-5-years-190524901581</t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Senior Developer</t>
+          <t>Service Management Senior Analyst</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-senior-developer-acronotics-pvt-ltd-pune-bengaluru-5-to-10-years-170524500545</t>
+          <t>https://www.naukri.com/job-listings-service-management-senior-analyst-accenture-solutions-pvt-ltd-chennai-5-to-8-years-180524908644</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Service Management Analyst</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-developer-acronotics-pvt-ltd-pune-bengaluru-3-to-8-years-170524500544</t>
+          <t>https://www.naukri.com/job-listings-service-management-analyst-accenture-solutions-pvt-ltd-chennai-3-to-5-years-180524904105</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Solution Architects</t>
+          <t>Service Management Associate</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-solution-architects-acronotics-pvt-ltd-pune-bengaluru-8-to-13-years-170524500638</t>
+          <t>https://www.naukri.com/job-listings-service-management-associate-accenture-solutions-pvt-ltd-bengaluru-1-to-3-years-190524903201</t>
         </is>
       </c>
     </row>
@@ -616,12 +616,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RPA  Robot Framework &amp; Python QA Automation</t>
+          <t>Application Developer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-rpa-robot-framework-python-qa-automation-rq-technologies-llp-chennai-5-to-10-years-170524011474</t>
+          <t>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-bengaluru-3-to-5-years-180524906353</t>
         </is>
       </c>
     </row>
@@ -631,12 +631,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Application Developer</t>
+          <t>Technology Architect</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-mumbai-3-to-5-years-170524908871</t>
+          <t>https://www.naukri.com/job-listings-technology-architect-accenture-solutions-pvt-ltd-bengaluru-12-to-16-years-190524903287</t>
         </is>
       </c>
     </row>
@@ -646,12 +646,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Application Developer</t>
+          <t>Business Analyst</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-3-to-6-years-170524904578</t>
+          <t>https://www.naukri.com/job-listings-business-analyst-accenture-solutions-pvt-ltd-pune-5-to-9-years-180524904126</t>
         </is>
       </c>
     </row>
@@ -661,12 +661,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Technical BotOps</t>
+          <t>Underwriting Specialist</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-technical-botops-allegis-group-hyderabad-1-to-5-years-170524004542</t>
+          <t>https://www.naukri.com/job-listings-underwriting-specialist-accenture-solutions-pvt-ltd-gurugram-7-to-11-years-180524903796</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Application Designer</t>
+          <t>SW/App/Cloud Tech Support Analyst</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-application-designer-accenture-solutions-pvt-ltd-bengaluru-3-to-5-years-170524912002</t>
+          <t>https://www.naukri.com/job-listings-sw-app-cloud-tech-support-analyst-accenture-solutions-pvt-ltd-hyderabad-3-to-5-years-180524907692</t>
         </is>
       </c>
     </row>
@@ -691,12 +691,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Application Designer</t>
+          <t>Service Management Associate</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-application-designer-accenture-solutions-pvt-ltd-bengaluru-3-to-7-years-170524911413</t>
+          <t>https://www.naukri.com/job-listings-service-management-associate-accenture-solutions-pvt-ltd-chennai-1-to-3-years-180524903797</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Application Designer</t>
+          <t>Data Analyst - IO - Client Reporting - Investment Data Management</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-application-designer-accenture-solutions-pvt-ltd-bengaluru-7-to-9-years-170524912884</t>
+          <t>https://www.naukri.com/job-listings-data-analyst-io-client-reporting-investment-data-management-m-amp-amp-amp-g-plc-mumbai-1-to-4-years-180524500057</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Trust &amp; Safety New Associate</t>
+          <t>Analyst - Revenue and Fixed assets profile</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-trust-safety-new-associate-accenture-solutions-pvt-ltd-gurugram-0-to-1-years-180524908538</t>
+          <t>https://www.naukri.com/job-listings-analyst-revenue-and-fixed-assets-profile-m-amp-amp-amp-g-plc-mumbai-1-to-3-years-180524500056</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>S&amp;C Global Network - Strategy - MC - Industry X - Capital Projects</t>
+          <t>Assistant Manager - Actuarial</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-s-c-global-network-strategy-mc-industry-x-capital-projects-accenture-solutions-pvt-ltd-gurugram-7-to-9-years-170524908957</t>
+          <t>https://www.naukri.com/job-listings-assistant-manager-actuarial-m-amp-amp-amp-g-plc-mumbai-3-to-5-years-180524500055</t>
         </is>
       </c>
     </row>

</xml_diff>